<commit_message>
Switch to captest_prototype alternative capacity testing framework; include paper and oral presentation
</commit_message>
<xml_diff>
--- a/data/Inventory.xlsx
+++ b/data/Inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JNEWM\Documents\DNV\Admin\PerformanceLead\AcceptanceTesting\BifiOutboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3E89B8-28ED-416A-972B-6F28B6AC5D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8391850-85D6-4CE9-9ECE-0CAC8251F414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A6FE89B3-6A49-4D44-8B22-AFB6DB9868D5}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>prj_file</t>
   </si>
@@ -236,6 +236,30 @@
   </si>
   <si>
     <t>GCR</t>
+  </si>
+  <si>
+    <t>sep</t>
+  </si>
+  <si>
+    <t>dayfirst</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Bifaciality</t>
+  </si>
+  <si>
+    <t>date_format</t>
+  </si>
+  <si>
+    <t>%m/%d/%y %H:%M</t>
+  </si>
+  <si>
+    <t>StrucShd</t>
+  </si>
+  <si>
+    <t>BakMismatch</t>
   </si>
 </sst>
 </file>
@@ -587,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0C0805-EEE6-4653-AC35-86306A08A792}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,12 +623,13 @@
     <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -627,16 +652,34 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
         <v>64</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
+      <c r="L1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -655,14 +698,32 @@
       <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" t="s">
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>43</v>
       </c>
+      <c r="L2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -684,14 +745,32 @@
       <c r="G3">
         <v>0.2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3">
+        <v>0.7</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>44</v>
       </c>
+      <c r="L3" t="s">
+        <v>68</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3">
+        <v>0.05</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -713,14 +792,32 @@
       <c r="G4">
         <v>0.2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4">
+        <v>0.7</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>45</v>
       </c>
+      <c r="L4" t="s">
+        <v>68</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4">
+        <v>0.05</v>
+      </c>
+      <c r="P4">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -742,14 +839,32 @@
       <c r="G5">
         <v>0.6</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5">
+        <v>0.7</v>
+      </c>
+      <c r="J5" t="s">
         <v>41</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>46</v>
       </c>
+      <c r="L5" t="s">
+        <v>68</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5">
+        <v>0.05</v>
+      </c>
+      <c r="P5">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -771,14 +886,32 @@
       <c r="G6">
         <v>0.6</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6">
+        <v>0.7</v>
+      </c>
+      <c r="J6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>47</v>
       </c>
+      <c r="L6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6">
+        <v>0.05</v>
+      </c>
+      <c r="P6">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -797,14 +930,32 @@
       <c r="F7" t="s">
         <v>60</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
         <v>21</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>53</v>
       </c>
+      <c r="L7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
@@ -827,16 +978,34 @@
         <v>0.2</v>
       </c>
       <c r="H8">
+        <v>0.7</v>
+      </c>
+      <c r="I8">
         <v>2</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>54</v>
       </c>
+      <c r="L8" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O8">
+        <v>0.05</v>
+      </c>
+      <c r="P8">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -859,13 +1028,31 @@
         <v>0.6</v>
       </c>
       <c r="H9">
+        <v>0.7</v>
+      </c>
+      <c r="I9">
         <v>2</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>41</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>55</v>
+      </c>
+      <c r="L9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9">
+        <v>0.05</v>
+      </c>
+      <c r="P9">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +1065,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80662E9B-D151-46C4-A2FA-77D7AAE13F23}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Z3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>